<commit_message>
feat(translations) : translations will now be made via node
</commit_message>
<xml_diff>
--- a/src/assets/translations/translations.xlsx
+++ b/src/assets/translations/translations.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="app|app.translation.json" sheetId="1" r:id="rId1"/>
+    <sheet name="src/assets/translations/transla" sheetId="1" r:id="rId1"/>
+    <sheet name="src/assets/translations/app/app" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -418,4 +419,54 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>key</v>
+      </c>
+      <c r="B1" t="str">
+        <v>de</v>
+      </c>
+      <c r="C1" t="str">
+        <v>fr</v>
+      </c>
+      <c r="D1" t="str">
+        <v>it</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>app.translation</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Deutsch</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Französisch</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Italienisch</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>app.title</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Title der App</v>
+      </c>
+      <c r="C3" t="str">
+        <v>titre du app</v>
+      </c>
+      <c r="D3" t="str">
+        <v>title des application</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor(translations): add es6 compatibility
</commit_message>
<xml_diff>
--- a/src/assets/translations/translations.xlsx
+++ b/src/assets/translations/translations.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="src/assets/translations/transla" sheetId="1" r:id="rId1"/>
-    <sheet name="src/assets/translations/app/app" sheetId="2" r:id="rId2"/>
+    <sheet name="src|assets\translations\transla" sheetId="1" r:id="rId1"/>
+    <sheet name="src|assets\translations\app\app" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>

<commit_message>
refactor(translations): create new translator
</commit_message>
<xml_diff>
--- a/src/assets/translations/translations.xlsx
+++ b/src/assets/translations/translations.xlsx
@@ -1,17 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\atw-seed\src\assets\translations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet name="src|assets\translations\transla" sheetId="1" r:id="rId1"/>
-    <sheet name="src|assets\translations\app\app" sheetId="2" r:id="rId2"/>
+    <sheet name="app1|app1.json" sheetId="1" r:id="rId1"/>
+    <sheet name="app2|app2.json" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>app.translation</t>
+  </si>
+  <si>
+    <t>Deutsch</t>
+  </si>
+  <si>
+    <t>Französisch</t>
+  </si>
+  <si>
+    <t>Italienisch</t>
+  </si>
+  <si>
+    <t>app.title</t>
+  </si>
+  <si>
+    <t>Title der App</t>
+  </si>
+  <si>
+    <t>titre du app</t>
+  </si>
+  <si>
+    <t>title des application</t>
+  </si>
+  <si>
+    <t>app2.translation</t>
+  </si>
+  <si>
+    <t>app2.title</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -44,10 +102,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -372,101 +438,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>key</v>
-      </c>
-      <c r="B1" t="str">
-        <v>de</v>
-      </c>
-      <c r="C1" t="str">
-        <v>fr</v>
-      </c>
-      <c r="D1" t="str">
-        <v>it</v>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>app.translation</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Deutsch</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Französisch</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Italienisch</v>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>app.title</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Title der App</v>
-      </c>
-      <c r="C3" t="str">
-        <v>titre du app</v>
-      </c>
-      <c r="D3" t="str">
-        <v>title des application</v>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>key</v>
-      </c>
-      <c r="B1" t="str">
-        <v>de</v>
-      </c>
-      <c r="C1" t="str">
-        <v>fr</v>
-      </c>
-      <c r="D1" t="str">
-        <v>it</v>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>app.translation</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Deutsch</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Französisch</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Italienisch</v>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>app.title</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Title der App</v>
-      </c>
-      <c r="C3" t="str">
-        <v>titre du app</v>
-      </c>
-      <c r="D3" t="str">
-        <v>title des application</v>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>